<commit_message>
Update POS analysis to work on MisInfoText
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/Fakespeak_POS_frequency.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/Fakespeak_POS_frequency.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_BC55316E4E848FFC3C953B997E944471223B8632" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/alp11_sfu_ca/Documents/SFU/2. Terms/09. 2025_Fall/Discourse Lab/Projects/fake_news_over_time/data/Fakespeak-ENG/Analysis_output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_C8983F56833A276046AB566CD3D293844F5823FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B65532A7-667D-415B-8ED3-9DDC2C67FEB5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -17,22 +22,30 @@
     <sheet name="counts_summary" sheetId="7" r:id="rId7"/>
     <sheet name="prop_summary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="22">
   <si>
     <t>POS</t>
   </si>
   <si>
-    <t>counts</t>
+    <t>count</t>
   </si>
   <si>
     <t>proportion</t>
@@ -47,10 +60,10 @@
     <t>PUNCT</t>
   </si>
   <si>
-    <t>PROPN</t>
+    <t>ADP</t>
   </si>
   <si>
-    <t>ADP</t>
+    <t>PROPN</t>
   </si>
   <si>
     <t>DET</t>
@@ -86,38 +99,20 @@
     <t>SYM</t>
   </si>
   <si>
+    <t>INTJ</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>INTJ</t>
-  </si>
-  <si>
-    <t>CONJ</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
+    <t>Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +124,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,11 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,13 +481,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,139 +500,175 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
+        <v>6652</v>
+      </c>
+      <c r="C2">
+        <v>0.17808952666523881</v>
+      </c>
+      <c r="E2" s="2">
         <v>6641</v>
       </c>
-      <c r="C2">
-        <v>0.17779503105590061</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
+        <v>4175</v>
+      </c>
+      <c r="C3">
+        <v>0.1117744699079032</v>
+      </c>
+      <c r="E3" s="2">
         <v>4168</v>
       </c>
-      <c r="C3">
-        <v>0.1115870636110516</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
+        <v>4112</v>
+      </c>
+      <c r="C4">
+        <v>0.11008781323623899</v>
+      </c>
+      <c r="E4" s="2">
         <v>4099</v>
       </c>
-      <c r="C4">
-        <v>0.1097397729706575</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
+        <v>3549</v>
+      </c>
+      <c r="C5">
+        <v>9.5014992503748119E-2</v>
+      </c>
+      <c r="E5" s="2">
         <v>3557</v>
       </c>
-      <c r="C5">
-        <v>9.5229171128721354E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
+        <v>3481</v>
+      </c>
+      <c r="C6">
+        <v>9.3194474191475696E-2</v>
+      </c>
+      <c r="E6" s="2">
         <v>3551</v>
       </c>
-      <c r="C6">
-        <v>9.5068537159991431E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
+        <v>2705</v>
+      </c>
+      <c r="C7">
+        <v>7.2419147569072612E-2</v>
+      </c>
+      <c r="E7" s="2">
         <v>2708</v>
       </c>
-      <c r="C7">
-        <v>7.2499464553437573E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
+        <v>2501</v>
+      </c>
+      <c r="C8">
+        <v>6.69575926322553E-2</v>
+      </c>
+      <c r="E8" s="2">
         <v>2502</v>
       </c>
-      <c r="C8">
-        <v>6.6984364960376949E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
+        <v>2217</v>
+      </c>
+      <c r="C9">
+        <v>5.9354251445705719E-2</v>
+      </c>
+      <c r="E9" s="2">
         <v>2175</v>
       </c>
-      <c r="C9">
-        <v>5.8229813664596272E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
+        <v>1920</v>
+      </c>
+      <c r="C10">
+        <v>5.1402869993574643E-2</v>
+      </c>
+      <c r="E10" s="2">
         <v>1915</v>
       </c>
-      <c r="C10">
-        <v>5.1269008352966383E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
+        <v>1229</v>
+      </c>
+      <c r="C11">
+        <v>3.2903191261512102E-2</v>
+      </c>
+      <c r="E11" s="2">
         <v>1217</v>
       </c>
-      <c r="C11">
-        <v>3.2581923324052263E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
+        <v>1089</v>
+      </c>
+      <c r="C12">
+        <v>2.915506532448062E-2</v>
+      </c>
+      <c r="E12" s="2">
         <v>1085</v>
       </c>
-      <c r="C12">
-        <v>2.9047976011993999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
+        <v>1033</v>
+      </c>
+      <c r="C13">
+        <v>2.7655814949668019E-2</v>
+      </c>
+      <c r="E13" s="2">
         <v>1055</v>
       </c>
-      <c r="C13">
-        <v>2.8244806168344402E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -637,52 +678,67 @@
       <c r="C14">
         <v>2.730777468408653E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="E14" s="2">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
+        <v>745</v>
+      </c>
+      <c r="C15">
+        <v>1.994538445063183E-2</v>
+      </c>
+      <c r="E15" s="2">
         <v>744</v>
       </c>
-      <c r="C15">
-        <v>1.9918612122510171E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
+        <v>679</v>
+      </c>
+      <c r="C16">
+        <v>1.8178410794602699E-2</v>
+      </c>
+      <c r="E16" s="2">
         <v>670</v>
       </c>
-      <c r="C16">
-        <v>1.7937459841507821E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
+        <v>137</v>
+      </c>
+      <c r="C17">
+        <v>3.6678089526665241E-3</v>
+      </c>
+      <c r="E17" s="2">
         <v>133</v>
       </c>
-      <c r="C17">
-        <v>3.5607196401799099E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>1.4992503748125941E-3</v>
+      </c>
+      <c r="E18" s="2">
         <v>60</v>
       </c>
-      <c r="C18">
-        <v>1.606339687299208E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -691,6 +747,19 @@
       </c>
       <c r="C19">
         <v>1.3921610623259799E-3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>37352</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>37352</v>
       </c>
     </row>
   </sheetData>
@@ -702,11 +771,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,117 +786,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>22970</v>
+        <v>23150</v>
       </c>
       <c r="C2">
-        <v>0.1655674487331964</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.1668648862940138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>15684</v>
+        <v>15741</v>
       </c>
       <c r="C3">
-        <v>0.1130500594658882</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>0.11346091469348039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>15448</v>
+        <v>15319</v>
       </c>
       <c r="C4">
-        <v>0.1113489746639276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.11041914441200849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>14936</v>
+        <v>14871</v>
       </c>
       <c r="C5">
-        <v>0.1076584856020471</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>0.107189966482863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>12701</v>
+        <v>12647</v>
       </c>
       <c r="C6">
-        <v>9.1548635888564531E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>9.1159404620319309E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>10212</v>
+        <v>10204</v>
       </c>
       <c r="C7">
-        <v>7.3607957617039685E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>7.3550293725447802E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>8740</v>
+        <v>8755</v>
       </c>
       <c r="C8">
-        <v>6.2997801564133066E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>6.3105921360867845E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>7905</v>
+        <v>7873</v>
       </c>
       <c r="C9">
-        <v>5.697913287923019E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5.6748477312862651E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>7367</v>
+        <v>7384</v>
       </c>
       <c r="C10">
-        <v>5.3101236169675999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>5.3223771939308752E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>4676</v>
+        <v>4701</v>
       </c>
       <c r="C11">
-        <v>3.3704544635456087E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>3.3884744296680723E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -838,81 +907,81 @@
         <v>3.054023858435146E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3514</v>
+      </c>
+      <c r="C13">
+        <v>2.5328864381734959E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>3555</v>
-      </c>
-      <c r="C13">
-        <v>2.5624391826143369E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
       <c r="B14">
-        <v>3505</v>
+        <v>3476</v>
       </c>
       <c r="C14">
-        <v>2.5263992503694089E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2.5054960896673511E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>3065</v>
+        <v>3127</v>
       </c>
       <c r="C15">
-        <v>2.2092478466140479E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2.253937362597758E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2669</v>
+        <v>2654</v>
       </c>
       <c r="C16">
-        <v>1.923811583234224E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1.9129996035607451E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>658</v>
+        <v>677</v>
       </c>
       <c r="C17">
-        <v>4.7428550834324431E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>4.8798068259631672E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>246</v>
+      </c>
+      <c r="C18">
+        <v>1.773164666450427E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>259</v>
-      </c>
-      <c r="C18">
-        <v>1.8668684902872379E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
       <c r="B19">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C19">
-        <v>1.066781994449851E-3</v>
+        <v>1.1460698453886909E-3</v>
       </c>
     </row>
   </sheetData>
@@ -924,11 +993,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,18 +1008,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>26692</v>
+        <v>26880</v>
       </c>
       <c r="C2">
-        <v>0.17731895755691521</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.17856786974111641</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -961,95 +1030,95 @@
         <v>0.1166204967747507</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>16357</v>
+        <v>16371</v>
       </c>
       <c r="C4">
-        <v>0.10866200317542569</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.10875500727424919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>14260</v>
+      </c>
+      <c r="C5">
+        <v>9.4731317801648826E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>14316</v>
-      </c>
-      <c r="C5">
-        <v>9.5103334196942821E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6">
-        <v>14242</v>
+        <v>14244</v>
       </c>
       <c r="C6">
-        <v>9.4611741103161479E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>9.4625027402993403E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>11522</v>
+        <v>11508</v>
       </c>
       <c r="C7">
-        <v>7.654237333173898E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>7.6449369232915482E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>9021</v>
+        <v>8908</v>
       </c>
       <c r="C8">
-        <v>5.9927855391912629E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>5.9177179451408678E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>8797</v>
+        <v>8791</v>
       </c>
       <c r="C9">
-        <v>5.8439789810736657E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5.8399930911240877E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>7557</v>
+        <v>7567</v>
       </c>
       <c r="C10">
-        <v>5.0202283914941109E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>5.0268715414100752E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>5087</v>
+        <v>5104</v>
       </c>
       <c r="C11">
-        <v>3.3793703622509649E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>3.3906637171081042E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1060,81 +1129,81 @@
         <v>2.8306461791923261E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>4082</v>
+        <v>4081</v>
       </c>
       <c r="C13">
-        <v>2.7117337956965679E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>2.7110694807049709E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>3982</v>
+        <v>3903</v>
       </c>
       <c r="C14">
-        <v>2.645302296536926E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2.5928214122008089E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>3497</v>
+        <v>3505</v>
       </c>
       <c r="C15">
-        <v>2.3231095256126641E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2.3284240455454359E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2766</v>
+        <v>2749</v>
       </c>
       <c r="C16">
-        <v>1.837495266755685E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1.8262019118985461E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>453</v>
+        <v>525</v>
       </c>
       <c r="C17">
-        <v>3.009346911931761E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>3.487653705881181E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>174</v>
+      </c>
+      <c r="C18">
+        <v>1.155908085377763E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>218</v>
-      </c>
-      <c r="C18">
-        <v>1.448206681680185E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
       <c r="B19">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="C19">
-        <v>8.3703688941148336E-4</v>
+        <v>9.6325673781480232E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1148,9 +1217,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,117 +1230,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>16320</v>
+        <v>16507</v>
       </c>
       <c r="C2">
-        <v>0.17821847050986639</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.18026055715112529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>10639</v>
+        <v>10649</v>
       </c>
       <c r="C3">
-        <v>0.1161805335633866</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>0.11628973605757149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>9725</v>
+        <v>9667</v>
       </c>
       <c r="C4">
-        <v>0.1061994255948806</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.1055660511286078</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>8714</v>
+      </c>
+      <c r="C5">
+        <v>9.5159053432780402E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>8722</v>
-      </c>
-      <c r="C5">
-        <v>9.5246415428128381E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6">
-        <v>8624</v>
+        <v>8568</v>
       </c>
       <c r="C6">
-        <v>9.4176230985115697E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>9.3564697017679888E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>6841</v>
+        <v>6823</v>
       </c>
       <c r="C7">
-        <v>7.4705426271936048E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>7.450886178240311E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>5619</v>
+        <v>5521</v>
       </c>
       <c r="C8">
-        <v>6.1360881482533061E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>6.0290697039520377E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>5234</v>
+        <v>5218</v>
       </c>
       <c r="C9">
-        <v>5.7156585456411828E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5.6981861465715877E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>4374</v>
+        <v>4389</v>
       </c>
       <c r="C10">
-        <v>4.7765170956504649E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>4.7928974697782102E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>3281</v>
+        <v>3256</v>
       </c>
       <c r="C11">
-        <v>3.5829338342087742E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>3.5556332106625323E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1351,7 @@
         <v>2.822884474681402E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1293,70 +1362,70 @@
         <v>2.700577681194238E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2392</v>
+        <v>2395</v>
       </c>
       <c r="C14">
-        <v>2.6121236609044151E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2.615399735729964E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2256</v>
+        <v>2228</v>
       </c>
       <c r="C15">
-        <v>2.4636082688128599E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2.4330315704410691E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>1683</v>
+        <v>1694</v>
       </c>
       <c r="C16">
-        <v>1.837877977132998E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1.8498902514933441E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>518</v>
+        <v>637</v>
       </c>
       <c r="C17">
-        <v>5.6566891987812999E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>6.9561988795824098E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>171</v>
+      </c>
+      <c r="C18">
+        <v>1.867362650562939E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>212</v>
-      </c>
-      <c r="C18">
-        <v>2.315092876721304E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
       <c r="B19">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C19">
-        <v>8.1901870638725384E-4</v>
+        <v>8.5177945464274402E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1370,9 +1439,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,106 +1452,106 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>21830</v>
+        <v>22107</v>
       </c>
       <c r="C2">
-        <v>0.18280326248974191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.18512284580214039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>13904</v>
+        <v>13934</v>
       </c>
       <c r="C3">
-        <v>0.11643135875663629</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>0.1166825771659214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>13075</v>
+        <v>12996</v>
       </c>
       <c r="C4">
-        <v>0.1094893567133933</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.108827814902276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>11914</v>
+      </c>
+      <c r="C5">
+        <v>9.9767204274062535E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>12022</v>
-      </c>
-      <c r="C5">
-        <v>0.1006715905474887</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6">
-        <v>11285</v>
+        <v>11261</v>
       </c>
       <c r="C6">
-        <v>9.449999162605302E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>9.4299016898624993E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>9163</v>
+        <v>9150</v>
       </c>
       <c r="C7">
-        <v>7.673047614262507E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>7.6621614831934887E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>7231</v>
+        <v>7131</v>
       </c>
       <c r="C8">
-        <v>6.0552010584668983E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>5.9714615887052201E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>6552</v>
+        <v>6500</v>
       </c>
       <c r="C9">
-        <v>5.4866100587851067E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5.4430655345090347E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>5565</v>
+        <v>5563</v>
       </c>
       <c r="C10">
-        <v>4.6601014922373507E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>4.6584267028421167E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1493,92 +1562,92 @@
         <v>3.2708636888911222E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>3690</v>
+        <v>3681</v>
       </c>
       <c r="C12">
-        <v>3.0899864342058981E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3.0824498819273481E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3139</v>
+        <v>3136</v>
       </c>
       <c r="C13">
-        <v>2.6285819558190562E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>2.6260697717262051E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>2978</v>
+        <v>2886</v>
       </c>
       <c r="C14">
-        <v>2.4937614095027549E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2.4167210973220121E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>2109</v>
+        <v>2129</v>
       </c>
       <c r="C15">
-        <v>1.766065417273778E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>1.782813311226113E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2090</v>
+        <v>2106</v>
       </c>
       <c r="C16">
-        <v>1.750154918019059E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1.763553233180927E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>576</v>
+        <v>749</v>
       </c>
       <c r="C17">
-        <v>4.8233934582726226E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>6.2720862851496422E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>189</v>
+      </c>
+      <c r="C18">
+        <v>1.5826759784957039E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>225</v>
-      </c>
-      <c r="C18">
-        <v>1.8841380696377431E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
       <c r="B19">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C19">
-        <v>6.5316786414108428E-4</v>
+        <v>6.6991575809341973E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1592,9 +1661,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1605,117 +1674,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4542</v>
+        <v>4612</v>
       </c>
       <c r="C2">
-        <v>0.16577852397985249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.16833345499671509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3272</v>
+        <v>3282</v>
       </c>
       <c r="C3">
-        <v>0.11942477553106071</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>0.1197897656763267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3088</v>
+        <v>3077</v>
       </c>
       <c r="C4">
-        <v>0.1127089568581648</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.1123074676983721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2991</v>
+      </c>
+      <c r="C5">
+        <v>0.1091685524490839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>3023</v>
-      </c>
-      <c r="C5">
-        <v>0.1103365209139353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6">
-        <v>2480</v>
+        <v>2465</v>
       </c>
       <c r="C6">
-        <v>9.0517556025987295E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>8.9970070808088179E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2065</v>
+        <v>2057</v>
       </c>
       <c r="C7">
-        <v>7.5370464997445069E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>7.5078472881232206E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1774</v>
+        <v>1758</v>
       </c>
       <c r="C8">
-        <v>6.4749251770202201E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>6.4165267537776474E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>1525</v>
+        <v>1537</v>
       </c>
       <c r="C9">
-        <v>5.5660997153076867E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5.6098985327396163E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="C10">
-        <v>4.8507190305861737E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>4.8616687349441558E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>920</v>
+        <v>879</v>
       </c>
       <c r="C11">
-        <v>3.3579093364479159E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>3.2082633768888237E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1726,81 +1795,81 @@
         <v>2.81407402000146E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>699</v>
+        <v>676</v>
       </c>
       <c r="C13">
-        <v>2.5512811154098841E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>2.4673333819986858E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C14">
-        <v>2.4089349587561131E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2.4198846631140958E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="C15">
-        <v>1.7008540769399231E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>1.7154536827505659E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C16">
-        <v>1.6643550624133151E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1.6680049638659759E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="C17">
-        <v>7.2998029053215566E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>1.021972406745018E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>1.788451711803781E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>91</v>
-      </c>
-      <c r="C18">
-        <v>3.3214103219213081E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
       <c r="B19">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C19">
-        <v>1.350463537484488E-3</v>
+        <v>1.5329586101175271E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1810,18 +1879,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -1830,37 +1902,37 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>18</v>
@@ -1869,382 +1941,361 @@
         <v>4</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2019</v>
       </c>
       <c r="B2">
-        <v>2175</v>
+        <v>2217</v>
       </c>
       <c r="C2">
-        <v>3551</v>
+        <v>3549</v>
       </c>
       <c r="D2">
-        <v>1217</v>
+        <v>1229</v>
       </c>
       <c r="E2">
-        <v>1915</v>
+        <v>1920</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1089</v>
       </c>
       <c r="G2">
-        <v>1085</v>
+        <v>2705</v>
       </c>
       <c r="H2">
-        <v>2708</v>
+        <v>56</v>
       </c>
       <c r="I2">
+        <v>6652</v>
+      </c>
+      <c r="J2">
+        <v>745</v>
+      </c>
+      <c r="K2">
+        <v>1033</v>
+      </c>
+      <c r="L2">
+        <v>2501</v>
+      </c>
+      <c r="M2">
+        <v>3481</v>
+      </c>
+      <c r="N2">
+        <v>4112</v>
+      </c>
+      <c r="O2">
+        <v>679</v>
+      </c>
+      <c r="P2">
+        <v>1020</v>
+      </c>
+      <c r="Q2">
+        <v>137</v>
+      </c>
+      <c r="R2">
+        <v>4175</v>
+      </c>
+      <c r="S2">
         <v>52</v>
       </c>
-      <c r="J2">
-        <v>6641</v>
-      </c>
-      <c r="K2">
-        <v>744</v>
-      </c>
-      <c r="L2">
-        <v>1055</v>
-      </c>
-      <c r="M2">
-        <v>2502</v>
-      </c>
-      <c r="N2">
-        <v>3557</v>
-      </c>
-      <c r="O2">
-        <v>4099</v>
-      </c>
-      <c r="P2">
-        <v>670</v>
-      </c>
-      <c r="Q2">
-        <v>133</v>
-      </c>
-      <c r="R2">
-        <v>4168</v>
-      </c>
-      <c r="S2">
-        <v>60</v>
-      </c>
-      <c r="T2">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2020</v>
       </c>
       <c r="B3">
-        <v>7905</v>
+        <v>7873</v>
       </c>
       <c r="C3">
-        <v>12701</v>
+        <v>12647</v>
       </c>
       <c r="D3">
-        <v>4676</v>
+        <v>4701</v>
       </c>
       <c r="E3">
-        <v>7367</v>
+        <v>7384</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>3514</v>
       </c>
       <c r="G3">
+        <v>10204</v>
+      </c>
+      <c r="H3">
+        <v>159</v>
+      </c>
+      <c r="I3">
+        <v>23150</v>
+      </c>
+      <c r="J3">
+        <v>3127</v>
+      </c>
+      <c r="K3">
+        <v>3476</v>
+      </c>
+      <c r="L3">
+        <v>8755</v>
+      </c>
+      <c r="M3">
+        <v>15319</v>
+      </c>
+      <c r="N3">
+        <v>15741</v>
+      </c>
+      <c r="O3">
+        <v>2654</v>
+      </c>
+      <c r="P3">
+        <v>4237</v>
+      </c>
+      <c r="Q3">
+        <v>677</v>
+      </c>
+      <c r="R3">
+        <v>14871</v>
+      </c>
+      <c r="S3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B4">
+        <v>8908</v>
+      </c>
+      <c r="C4">
+        <v>14244</v>
+      </c>
+      <c r="D4">
+        <v>5104</v>
+      </c>
+      <c r="E4">
+        <v>7567</v>
+      </c>
+      <c r="F4">
+        <v>4081</v>
+      </c>
+      <c r="G4">
+        <v>11508</v>
+      </c>
+      <c r="H4">
+        <v>145</v>
+      </c>
+      <c r="I4">
+        <v>26880</v>
+      </c>
+      <c r="J4">
         <v>3505</v>
       </c>
-      <c r="H3">
-        <v>10212</v>
-      </c>
-      <c r="I3">
-        <v>148</v>
-      </c>
-      <c r="J3">
-        <v>22970</v>
-      </c>
-      <c r="K3">
-        <v>3065</v>
-      </c>
-      <c r="L3">
-        <v>3555</v>
-      </c>
-      <c r="M3">
-        <v>8740</v>
-      </c>
-      <c r="N3">
-        <v>15448</v>
-      </c>
-      <c r="O3">
-        <v>15684</v>
-      </c>
-      <c r="P3">
-        <v>2669</v>
-      </c>
-      <c r="Q3">
-        <v>658</v>
-      </c>
-      <c r="R3">
-        <v>14936</v>
-      </c>
-      <c r="S3">
-        <v>259</v>
-      </c>
-      <c r="T3">
-        <v>4237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>9021</v>
-      </c>
-      <c r="C4">
-        <v>14242</v>
-      </c>
-      <c r="D4">
-        <v>5087</v>
-      </c>
-      <c r="E4">
-        <v>7557</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>4082</v>
-      </c>
-      <c r="H4">
-        <v>11522</v>
-      </c>
-      <c r="I4">
-        <v>126</v>
-      </c>
-      <c r="J4">
-        <v>26692</v>
-      </c>
       <c r="K4">
-        <v>3497</v>
+        <v>3903</v>
       </c>
       <c r="L4">
-        <v>3982</v>
+        <v>8791</v>
       </c>
       <c r="M4">
-        <v>8797</v>
+        <v>14260</v>
       </c>
       <c r="N4">
-        <v>14316</v>
+        <v>17555</v>
       </c>
       <c r="O4">
-        <v>17555</v>
+        <v>2749</v>
       </c>
       <c r="P4">
-        <v>2766</v>
+        <v>4261</v>
       </c>
       <c r="Q4">
-        <v>453</v>
+        <v>525</v>
       </c>
       <c r="R4">
-        <v>16357</v>
+        <v>16371</v>
       </c>
       <c r="S4">
-        <v>218</v>
-      </c>
-      <c r="T4">
-        <v>4261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2022</v>
       </c>
       <c r="B5">
-        <v>5619</v>
+        <v>5521</v>
       </c>
       <c r="C5">
-        <v>8722</v>
+        <v>8714</v>
       </c>
       <c r="D5">
-        <v>3281</v>
+        <v>3256</v>
       </c>
       <c r="E5">
-        <v>4374</v>
+        <v>4389</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2395</v>
       </c>
       <c r="G5">
-        <v>2392</v>
+        <v>6823</v>
       </c>
       <c r="H5">
-        <v>6841</v>
+        <v>78</v>
       </c>
       <c r="I5">
-        <v>75</v>
+        <v>16507</v>
       </c>
       <c r="J5">
-        <v>16320</v>
+        <v>2473</v>
       </c>
       <c r="K5">
-        <v>2473</v>
+        <v>2228</v>
       </c>
       <c r="L5">
-        <v>2256</v>
+        <v>5218</v>
       </c>
       <c r="M5">
-        <v>5234</v>
+        <v>8568</v>
       </c>
       <c r="N5">
-        <v>8624</v>
+        <v>10649</v>
       </c>
       <c r="O5">
-        <v>10639</v>
+        <v>1694</v>
       </c>
       <c r="P5">
-        <v>1683</v>
+        <v>2585</v>
       </c>
       <c r="Q5">
-        <v>518</v>
+        <v>637</v>
       </c>
       <c r="R5">
-        <v>9725</v>
+        <v>9667</v>
       </c>
       <c r="S5">
-        <v>212</v>
-      </c>
-      <c r="T5">
-        <v>2585</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2023</v>
       </c>
       <c r="B6">
-        <v>7231</v>
+        <v>7131</v>
       </c>
       <c r="C6">
-        <v>11285</v>
+        <v>11261</v>
       </c>
       <c r="D6">
-        <v>3690</v>
+        <v>3681</v>
       </c>
       <c r="E6">
-        <v>5565</v>
+        <v>5563</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3136</v>
       </c>
       <c r="G6">
-        <v>3139</v>
+        <v>9150</v>
       </c>
       <c r="H6">
-        <v>9163</v>
+        <v>80</v>
       </c>
       <c r="I6">
-        <v>78</v>
+        <v>22107</v>
       </c>
       <c r="J6">
-        <v>21830</v>
+        <v>2129</v>
       </c>
       <c r="K6">
-        <v>2109</v>
+        <v>2886</v>
       </c>
       <c r="L6">
-        <v>2978</v>
+        <v>6500</v>
       </c>
       <c r="M6">
-        <v>6552</v>
+        <v>11914</v>
       </c>
       <c r="N6">
-        <v>12022</v>
+        <v>13934</v>
       </c>
       <c r="O6">
-        <v>13904</v>
+        <v>2106</v>
       </c>
       <c r="P6">
-        <v>2090</v>
+        <v>3906</v>
       </c>
       <c r="Q6">
-        <v>576</v>
+        <v>749</v>
       </c>
       <c r="R6">
-        <v>13075</v>
+        <v>12996</v>
       </c>
       <c r="S6">
-        <v>225</v>
-      </c>
-      <c r="T6">
-        <v>3906</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2024</v>
       </c>
       <c r="B7">
-        <v>1525</v>
+        <v>1537</v>
       </c>
       <c r="C7">
-        <v>2480</v>
+        <v>2465</v>
       </c>
       <c r="D7">
-        <v>920</v>
+        <v>879</v>
       </c>
       <c r="E7">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>663</v>
       </c>
       <c r="G7">
-        <v>660</v>
+        <v>2057</v>
       </c>
       <c r="H7">
-        <v>2065</v>
+        <v>42</v>
       </c>
       <c r="I7">
-        <v>37</v>
+        <v>4612</v>
       </c>
       <c r="J7">
-        <v>4542</v>
+        <v>457</v>
       </c>
       <c r="K7">
-        <v>456</v>
+        <v>676</v>
       </c>
       <c r="L7">
-        <v>699</v>
+        <v>1758</v>
       </c>
       <c r="M7">
-        <v>1774</v>
+        <v>2991</v>
       </c>
       <c r="N7">
-        <v>3023</v>
+        <v>3282</v>
       </c>
       <c r="O7">
-        <v>3272</v>
+        <v>470</v>
       </c>
       <c r="P7">
-        <v>466</v>
+        <v>771</v>
       </c>
       <c r="Q7">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="R7">
-        <v>3088</v>
+        <v>3077</v>
       </c>
       <c r="S7">
-        <v>91</v>
-      </c>
-      <c r="T7">
-        <v>771</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2254,18 +2305,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -2274,37 +2328,37 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>18</v>
@@ -2313,382 +2367,361 @@
         <v>4</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2019</v>
       </c>
       <c r="B2">
-        <v>5.8229813664596272E-2</v>
+        <v>5.9354251445705719E-2</v>
       </c>
       <c r="C2">
-        <v>9.5068537159991431E-2</v>
+        <v>9.5014992503748119E-2</v>
       </c>
       <c r="D2">
-        <v>3.2581923324052263E-2</v>
+        <v>3.2903191261512102E-2</v>
       </c>
       <c r="E2">
-        <v>5.1269008352966383E-2</v>
+        <v>5.1402869993574643E-2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2.915506532448062E-2</v>
       </c>
       <c r="G2">
-        <v>2.9047976011993999E-2</v>
+        <v>7.2419147569072612E-2</v>
       </c>
       <c r="H2">
-        <v>7.2499464553437573E-2</v>
+        <v>1.4992503748125941E-3</v>
       </c>
       <c r="I2">
+        <v>0.17808952666523881</v>
+      </c>
+      <c r="J2">
+        <v>1.994538445063183E-2</v>
+      </c>
+      <c r="K2">
+        <v>2.7655814949668019E-2</v>
+      </c>
+      <c r="L2">
+        <v>6.69575926322553E-2</v>
+      </c>
+      <c r="M2">
+        <v>9.3194474191475696E-2</v>
+      </c>
+      <c r="N2">
+        <v>0.11008781323623899</v>
+      </c>
+      <c r="O2">
+        <v>1.8178410794602699E-2</v>
+      </c>
+      <c r="P2">
+        <v>2.730777468408653E-2</v>
+      </c>
+      <c r="Q2">
+        <v>3.6678089526665241E-3</v>
+      </c>
+      <c r="R2">
+        <v>0.1117744699079032</v>
+      </c>
+      <c r="S2">
         <v>1.3921610623259799E-3</v>
       </c>
-      <c r="J2">
-        <v>0.17779503105590061</v>
-      </c>
-      <c r="K2">
-        <v>1.9918612122510171E-2</v>
-      </c>
-      <c r="L2">
-        <v>2.8244806168344402E-2</v>
-      </c>
-      <c r="M2">
-        <v>6.6984364960376949E-2</v>
-      </c>
-      <c r="N2">
-        <v>9.5229171128721354E-2</v>
-      </c>
-      <c r="O2">
-        <v>0.1097397729706575</v>
-      </c>
-      <c r="P2">
-        <v>1.7937459841507821E-2</v>
-      </c>
-      <c r="Q2">
-        <v>3.5607196401799099E-3</v>
-      </c>
-      <c r="R2">
-        <v>0.1115870636110516</v>
-      </c>
-      <c r="S2">
-        <v>1.606339687299208E-3</v>
-      </c>
-      <c r="T2">
-        <v>2.730777468408653E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2020</v>
       </c>
       <c r="B3">
-        <v>5.697913287923019E-2</v>
+        <v>5.6748477312862651E-2</v>
       </c>
       <c r="C3">
-        <v>9.1548635888564531E-2</v>
+        <v>9.1159404620319309E-2</v>
       </c>
       <c r="D3">
-        <v>3.3704544635456087E-2</v>
+        <v>3.3884744296680723E-2</v>
       </c>
       <c r="E3">
-        <v>5.3101236169675999E-2</v>
+        <v>5.3223771939308752E-2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2.5328864381734959E-2</v>
       </c>
       <c r="G3">
-        <v>2.5263992503694089E-2</v>
+        <v>7.3550293725447802E-2</v>
       </c>
       <c r="H3">
-        <v>7.3607957617039685E-2</v>
+        <v>1.1460698453886909E-3</v>
       </c>
       <c r="I3">
-        <v>1.066781994449851E-3</v>
+        <v>0.1668648862940138</v>
       </c>
       <c r="J3">
-        <v>0.1655674487331964</v>
+        <v>2.253937362597758E-2</v>
       </c>
       <c r="K3">
-        <v>2.2092478466140479E-2</v>
+        <v>2.5054960896673511E-2</v>
       </c>
       <c r="L3">
-        <v>2.5624391826143369E-2</v>
+        <v>6.3105921360867845E-2</v>
       </c>
       <c r="M3">
-        <v>6.2997801564133066E-2</v>
+        <v>0.11041914441200849</v>
       </c>
       <c r="N3">
-        <v>0.1113489746639276</v>
+        <v>0.11346091469348039</v>
       </c>
       <c r="O3">
-        <v>0.1130500594658882</v>
+        <v>1.9129996035607451E-2</v>
       </c>
       <c r="P3">
-        <v>1.923811583234224E-2</v>
+        <v>3.054023858435146E-2</v>
       </c>
       <c r="Q3">
-        <v>4.7428550834324431E-3</v>
+        <v>4.8798068259631672E-3</v>
       </c>
       <c r="R3">
-        <v>0.1076584856020471</v>
+        <v>0.107189966482863</v>
       </c>
       <c r="S3">
-        <v>1.8668684902872379E-3</v>
-      </c>
-      <c r="T3">
-        <v>3.054023858435146E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>1.773164666450427E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2021</v>
       </c>
       <c r="B4">
-        <v>5.9927855391912629E-2</v>
+        <v>5.9177179451408678E-2</v>
       </c>
       <c r="C4">
-        <v>9.4611741103161479E-2</v>
+        <v>9.4625027402993403E-2</v>
       </c>
       <c r="D4">
-        <v>3.3793703622509649E-2</v>
+        <v>3.3906637171081042E-2</v>
       </c>
       <c r="E4">
-        <v>5.0202283914941109E-2</v>
+        <v>5.0268715414100752E-2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2.7110694807049709E-2</v>
       </c>
       <c r="G4">
-        <v>2.7117337956965679E-2</v>
+        <v>7.6449369232915482E-2</v>
       </c>
       <c r="H4">
-        <v>7.654237333173898E-2</v>
+        <v>9.6325673781480232E-4</v>
       </c>
       <c r="I4">
-        <v>8.3703688941148336E-4</v>
+        <v>0.17856786974111641</v>
       </c>
       <c r="J4">
-        <v>0.17731895755691521</v>
+        <v>2.3284240455454359E-2</v>
       </c>
       <c r="K4">
-        <v>2.3231095256126641E-2</v>
+        <v>2.5928214122008089E-2</v>
       </c>
       <c r="L4">
-        <v>2.645302296536926E-2</v>
+        <v>5.8399930911240877E-2</v>
       </c>
       <c r="M4">
-        <v>5.8439789810736657E-2</v>
+        <v>9.4731317801648826E-2</v>
       </c>
       <c r="N4">
-        <v>9.5103334196942821E-2</v>
+        <v>0.1166204967747507</v>
       </c>
       <c r="O4">
-        <v>0.1166204967747507</v>
+        <v>1.8262019118985461E-2</v>
       </c>
       <c r="P4">
-        <v>1.837495266755685E-2</v>
+        <v>2.8306461791923261E-2</v>
       </c>
       <c r="Q4">
-        <v>3.009346911931761E-3</v>
+        <v>3.487653705881181E-3</v>
       </c>
       <c r="R4">
-        <v>0.10866200317542569</v>
+        <v>0.10875500727424919</v>
       </c>
       <c r="S4">
-        <v>1.448206681680185E-3</v>
-      </c>
-      <c r="T4">
-        <v>2.8306461791923261E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>1.155908085377763E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2022</v>
       </c>
       <c r="B5">
-        <v>6.1360881482533061E-2</v>
+        <v>6.0290697039520377E-2</v>
       </c>
       <c r="C5">
-        <v>9.5246415428128381E-2</v>
+        <v>9.5159053432780402E-2</v>
       </c>
       <c r="D5">
-        <v>3.5829338342087742E-2</v>
+        <v>3.5556332106625323E-2</v>
       </c>
       <c r="E5">
-        <v>4.7765170956504649E-2</v>
+        <v>4.7928974697782102E-2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2.615399735729964E-2</v>
       </c>
       <c r="G5">
-        <v>2.6121236609044151E-2</v>
+        <v>7.450886178240311E-2</v>
       </c>
       <c r="H5">
-        <v>7.4705426271936048E-2</v>
+        <v>8.5177945464274402E-4</v>
       </c>
       <c r="I5">
-        <v>8.1901870638725384E-4</v>
+        <v>0.18026055715112529</v>
       </c>
       <c r="J5">
-        <v>0.17821847050986639</v>
+        <v>2.700577681194238E-2</v>
       </c>
       <c r="K5">
-        <v>2.700577681194238E-2</v>
+        <v>2.4330315704410691E-2</v>
       </c>
       <c r="L5">
-        <v>2.4636082688128599E-2</v>
+        <v>5.6981861465715877E-2</v>
       </c>
       <c r="M5">
-        <v>5.7156585456411828E-2</v>
+        <v>9.3564697017679888E-2</v>
       </c>
       <c r="N5">
-        <v>9.4176230985115697E-2</v>
+        <v>0.11628973605757149</v>
       </c>
       <c r="O5">
-        <v>0.1161805335633866</v>
+        <v>1.8498902514933441E-2</v>
       </c>
       <c r="P5">
-        <v>1.837877977132998E-2</v>
+        <v>2.822884474681402E-2</v>
       </c>
       <c r="Q5">
-        <v>5.6566891987812999E-3</v>
+        <v>6.9561988795824098E-3</v>
       </c>
       <c r="R5">
-        <v>0.1061994255948806</v>
+        <v>0.1055660511286078</v>
       </c>
       <c r="S5">
-        <v>2.315092876721304E-3</v>
-      </c>
-      <c r="T5">
-        <v>2.822884474681402E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>1.867362650562939E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2023</v>
       </c>
       <c r="B6">
-        <v>6.0552010584668983E-2</v>
+        <v>5.9714615887052201E-2</v>
       </c>
       <c r="C6">
-        <v>9.449999162605302E-2</v>
+        <v>9.4299016898624993E-2</v>
       </c>
       <c r="D6">
-        <v>3.0899864342058981E-2</v>
+        <v>3.0824498819273481E-2</v>
       </c>
       <c r="E6">
-        <v>4.6601014922373507E-2</v>
+        <v>4.6584267028421167E-2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2.6260697717262051E-2</v>
       </c>
       <c r="G6">
-        <v>2.6285819558190562E-2</v>
+        <v>7.6621614831934887E-2</v>
       </c>
       <c r="H6">
-        <v>7.673047614262507E-2</v>
+        <v>6.6991575809341973E-4</v>
       </c>
       <c r="I6">
-        <v>6.5316786414108428E-4</v>
+        <v>0.18512284580214039</v>
       </c>
       <c r="J6">
-        <v>0.18280326248974191</v>
+        <v>1.782813311226113E-2</v>
       </c>
       <c r="K6">
-        <v>1.766065417273778E-2</v>
+        <v>2.4167210973220121E-2</v>
       </c>
       <c r="L6">
-        <v>2.4937614095027549E-2</v>
+        <v>5.4430655345090347E-2</v>
       </c>
       <c r="M6">
-        <v>5.4866100587851067E-2</v>
+        <v>9.9767204274062535E-2</v>
       </c>
       <c r="N6">
-        <v>0.1006715905474887</v>
+        <v>0.1166825771659214</v>
       </c>
       <c r="O6">
-        <v>0.11643135875663629</v>
+        <v>1.763553233180927E-2</v>
       </c>
       <c r="P6">
-        <v>1.750154918019059E-2</v>
+        <v>3.2708636888911222E-2</v>
       </c>
       <c r="Q6">
-        <v>4.8233934582726226E-3</v>
+        <v>6.2720862851496422E-3</v>
       </c>
       <c r="R6">
-        <v>0.1094893567133933</v>
+        <v>0.108827814902276</v>
       </c>
       <c r="S6">
-        <v>1.8841380696377431E-3</v>
-      </c>
-      <c r="T6">
-        <v>3.2708636888911222E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>1.5826759784957039E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2024</v>
       </c>
       <c r="B7">
-        <v>5.5660997153076867E-2</v>
+        <v>5.6098985327396163E-2</v>
       </c>
       <c r="C7">
-        <v>9.0517556025987295E-2</v>
+        <v>8.9970070808088179E-2</v>
       </c>
       <c r="D7">
-        <v>3.3579093364479159E-2</v>
+        <v>3.2082633768888237E-2</v>
       </c>
       <c r="E7">
-        <v>4.8507190305861737E-2</v>
+        <v>4.8616687349441558E-2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2.4198846631140958E-2</v>
       </c>
       <c r="G7">
-        <v>2.4089349587561131E-2</v>
+        <v>7.5078472881232206E-2</v>
       </c>
       <c r="H7">
-        <v>7.5370464997445069E-2</v>
+        <v>1.5329586101175271E-3</v>
       </c>
       <c r="I7">
-        <v>1.350463537484488E-3</v>
+        <v>0.16833345499671509</v>
       </c>
       <c r="J7">
-        <v>0.16577852397985249</v>
+        <v>1.6680049638659759E-2</v>
       </c>
       <c r="K7">
-        <v>1.6643550624133151E-2</v>
+        <v>2.4673333819986858E-2</v>
       </c>
       <c r="L7">
-        <v>2.5512811154098841E-2</v>
+        <v>6.4165267537776474E-2</v>
       </c>
       <c r="M7">
-        <v>6.4749251770202201E-2</v>
+        <v>0.1091685524490839</v>
       </c>
       <c r="N7">
-        <v>0.1103365209139353</v>
+        <v>0.1197897656763267</v>
       </c>
       <c r="O7">
-        <v>0.11942477553106071</v>
+        <v>1.7154536827505659E-2</v>
       </c>
       <c r="P7">
-        <v>1.7008540769399231E-2</v>
+        <v>2.81407402000146E-2</v>
       </c>
       <c r="Q7">
-        <v>7.2998029053215566E-3</v>
+        <v>1.021972406745018E-2</v>
       </c>
       <c r="R7">
-        <v>0.1127089568581648</v>
+        <v>0.1123074676983721</v>
       </c>
       <c r="S7">
-        <v>3.3214103219213081E-3</v>
-      </c>
-      <c r="T7">
-        <v>2.81407402000146E-2</v>
+        <v>1.788451711803781E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>